<commit_message>
KIBON-605: Das Kindergarten-Flag fehlt auf der Statistik "Institutionen"
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egch\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7EFD38-0457-4080-A7B3-C9A12A6E3DEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE024CCF-43C8-4330-8D08-E58FD3913A5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>{anschrift}</t>
+  </si>
+  <si>
+    <t>{kindergartenTitle}</t>
+  </si>
+  <si>
+    <t>{isKindergarten}</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -556,20 +562,20 @@
     <col min="10" max="10" width="33.5703125" customWidth="1"/>
     <col min="11" max="11" width="24.5703125" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="13" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="24.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -610,22 +616,25 @@
         <v>28</v>
       </c>
       <c r="N4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -666,21 +675,24 @@
         <v>13</v>
       </c>
       <c r="N5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-1462 Institutionen Report ergänzt, kleine Korrekturen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egch\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE024CCF-43C8-4330-8D08-E58FD3913A5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBA4275-8F18-4430-B911-3A574ECA7424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="29400" yWindow="1320" windowWidth="21600" windowHeight="12735" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>{isKindergarten}</t>
+  </si>
+  <si>
+    <t>{oeffnungstageTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungstage}</t>
+  </si>
+  <si>
+    <t>{oeffnungsAbweichungen}</t>
+  </si>
+  <si>
+    <t>{oeffnungsAbweichungenTitle}</t>
   </si>
 </sst>
 </file>
@@ -544,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,23 +571,24 @@
     <col min="7" max="7" width="27.85546875" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" customWidth="1"/>
-    <col min="13" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="24.7109375" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="10" max="11" width="33.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -607,34 +620,40 @@
         <v>25</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="U4" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -666,33 +685,39 @@
         <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="U5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-1721 add gueltig ab / gueltig bis to institutionen report
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBA4275-8F18-4430-B911-3A574ECA7424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAEDD4-603C-4A1B-A566-61CE6C3F2017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="1320" windowWidth="21600" windowHeight="12735" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="30705" yWindow="1905" windowWidth="21600" windowHeight="12675" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>{oeffnungsAbweichungenTitle}</t>
+  </si>
+  <si>
+    <t>{gueltigAbTitle}</t>
+  </si>
+  <si>
+    <t>{gueltigAb}</t>
+  </si>
+  <si>
+    <t>{gueltigBisTitle}</t>
+  </si>
+  <si>
+    <t>{gueltigBis}</t>
   </si>
 </sst>
 </file>
@@ -556,7 +568,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -571,24 +583,24 @@
     <col min="7" max="7" width="27.85546875" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="11" width="33.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="24.5703125" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" customWidth="1"/>
-    <col min="15" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" customWidth="1"/>
-    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="10" max="13" width="33.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" customWidth="1"/>
+    <col min="17" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="24.7109375" customWidth="1"/>
+    <col min="23" max="23" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -623,37 +635,43 @@
         <v>40</v>
       </c>
       <c r="L4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="U4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="V4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="W4" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -687,37 +705,43 @@
       <c r="K5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="V5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="W5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-129: adapt test setups with gesuchperiode that are persisted
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAEDD4-603C-4A1B-A566-61CE6C3F2017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817CE342-4B7E-4B17-BD43-FC00330408A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="1905" windowWidth="21600" windowHeight="12675" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -66,9 +66,6 @@
     <t>{url}</t>
   </si>
   <si>
-    <t>{oeffnungszeiten}</t>
-  </si>
-  <si>
     <t>{isBaby}</t>
   </si>
   <si>
@@ -90,91 +87,196 @@
     <t>{zuletztGeaendert}</t>
   </si>
   <si>
+    <t>{typTitle}</t>
+  </si>
+  <si>
+    <t>{strasseTitle}</t>
+  </si>
+  <si>
+    <t>{plzTitle}</t>
+  </si>
+  <si>
+    <t>{ortTitle}</t>
+  </si>
+  <si>
+    <t>{telefonTitle}</t>
+  </si>
+  <si>
+    <t>{urlTitle}</t>
+  </si>
+  <si>
+    <t>{babyTitle}</t>
+  </si>
+  <si>
+    <t>{vorschulkindTitle}</t>
+  </si>
+  <si>
+    <t>{schulkindTitle}</t>
+  </si>
+  <si>
+    <t>{subventioniertTitle}</t>
+  </si>
+  <si>
+    <t>{kapazitaetTitle}</t>
+  </si>
+  <si>
+    <t>{reserviertFuerFirmenTitle}</t>
+  </si>
+  <si>
+    <t>{zuletztGeaendertTitle}</t>
+  </si>
+  <si>
+    <t>{nameTitle}</t>
+  </si>
+  <si>
+    <t>{name}</t>
+  </si>
+  <si>
+    <t>{anschriftTitle}</t>
+  </si>
+  <si>
+    <t>{anschrift}</t>
+  </si>
+  <si>
+    <t>{kindergartenTitle}</t>
+  </si>
+  <si>
+    <t>{isKindergarten}</t>
+  </si>
+  <si>
+    <t>{oeffnungstageTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungstage}</t>
+  </si>
+  <si>
+    <t>{oeffnungsAbweichungen}</t>
+  </si>
+  <si>
+    <t>{oeffnungsAbweichungenTitle}</t>
+  </si>
+  <si>
+    <t>{gueltigAbTitle}</t>
+  </si>
+  <si>
+    <t>{gueltigAb}</t>
+  </si>
+  <si>
+    <t>{gueltigBisTitle}</t>
+  </si>
+  <si>
+    <t>{gueltigBis}</t>
+  </si>
+  <si>
+    <t>{traegerschaftEmailTitle}</t>
+  </si>
+  <si>
+    <t>{traegerschaftEmail}</t>
+  </si>
+  <si>
+    <t>{familienportalEmailTitle}</t>
+  </si>
+  <si>
+    <t>{familienportalEmail}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBonTitle}</t>
+  </si>
+  <si>
+    <t>{gemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{bfsGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{bfsGemeinde}</t>
+  </si>
+  <si>
+    <t>{oeffnungstageProJahrTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungstageProJahr}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitAbTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitAb}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitBisTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitBis}</t>
+  </si>
+  <si>
+    <t>{summePensumWarteliste}</t>
+  </si>
+  <si>
+    <t>{anzahlKinderWartelisteTitle}</t>
+  </si>
+  <si>
+    <t>{anzahlKinderWarteliste}</t>
+  </si>
+  <si>
+    <t>{auslastungTitle}</t>
+  </si>
+  <si>
+    <t>{auslastung}</t>
+  </si>
+  <si>
+    <t>{summePensumWartelisteTitle}</t>
+  </si>
+  <si>
+    <t>{dauerWartelisteTitle}</t>
+  </si>
+  <si>
+    <t>{dauerWarteliste}</t>
+  </si>
+  <si>
+    <t>{grundSchliessungTitle}</t>
+  </si>
+  <si>
+    <t>{grundSchliessung}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBon}</t>
+  </si>
+  <si>
     <t>{repeatInstitutionenRow}</t>
   </si>
   <si>
-    <t>{typTitle}</t>
-  </si>
-  <si>
-    <t>{strasseTitle}</t>
-  </si>
-  <si>
-    <t>{plzTitle}</t>
-  </si>
-  <si>
-    <t>{ortTitle}</t>
-  </si>
-  <si>
-    <t>{telefonTitle}</t>
-  </si>
-  <si>
-    <t>{urlTitle}</t>
-  </si>
-  <si>
-    <t>{oeffnungszeitenTitle}</t>
-  </si>
-  <si>
-    <t>{babyTitle}</t>
-  </si>
-  <si>
-    <t>{vorschulkindTitle}</t>
-  </si>
-  <si>
-    <t>{schulkindTitle}</t>
-  </si>
-  <si>
-    <t>{subventioniertTitle}</t>
-  </si>
-  <si>
-    <t>{kapazitaetTitle}</t>
-  </si>
-  <si>
-    <t>{reserviertFuerFirmenTitle}</t>
-  </si>
-  <si>
-    <t>{zuletztGeaendertTitle}</t>
-  </si>
-  <si>
-    <t>{nameTitle}</t>
-  </si>
-  <si>
-    <t>{name}</t>
-  </si>
-  <si>
-    <t>{anschriftTitle}</t>
-  </si>
-  <si>
-    <t>{anschrift}</t>
-  </si>
-  <si>
-    <t>{kindergartenTitle}</t>
-  </si>
-  <si>
-    <t>{isKindergarten}</t>
-  </si>
-  <si>
-    <t>{oeffnungstageTitle}</t>
-  </si>
-  <si>
-    <t>{oeffnungstage}</t>
-  </si>
-  <si>
-    <t>{oeffnungsAbweichungen}</t>
-  </si>
-  <si>
-    <t>{oeffnungsAbweichungenTitle}</t>
-  </si>
-  <si>
-    <t>{gueltigAbTitle}</t>
-  </si>
-  <si>
-    <t>{gueltigAb}</t>
-  </si>
-  <si>
-    <t>{gueltigBisTitle}</t>
-  </si>
-  <si>
-    <t>{gueltigBis}</t>
+    <t>{oeffnungAnWochenenden}</t>
+  </si>
+  <si>
+    <t>{uebernachtungMoeglich}</t>
+  </si>
+  <si>
+    <t>{uebernachtungMoeglichTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungAnWochenendenTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungVorTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungVor}</t>
+  </si>
+  <si>
+    <t>{oeffnungNachTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungNach}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBonMail}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBonMailTitle}</t>
   </si>
 </sst>
 </file>
@@ -212,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -235,16 +337,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -254,6 +375,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -568,181 +695,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="13" width="33.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" customWidth="1"/>
-    <col min="17" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="22" width="24.7109375" customWidth="1"/>
-    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="2" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="12" max="14" width="27.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="21" width="33.5703125" customWidth="1"/>
+    <col min="22" max="25" width="20.140625" customWidth="1"/>
+    <col min="26" max="27" width="38" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.5703125" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="L4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="J5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="5" t="s">
+      <c r="AF5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="5" t="s">
+      <c r="AG5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="AH5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="AI5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>19</v>
+      <c r="AK5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO5" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2046: add new fields to insti statistik vorlage
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAEDD4-603C-4A1B-A566-61CE6C3F2017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67AAF81-4436-45FA-8B08-40A31AFE7406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="1905" windowWidth="21600" windowHeight="12675" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -66,9 +66,6 @@
     <t>{url}</t>
   </si>
   <si>
-    <t>{oeffnungszeiten}</t>
-  </si>
-  <si>
     <t>{isBaby}</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>{zuletztGeaendert}</t>
   </si>
   <si>
-    <t>{repeatInstitutionenRow}</t>
-  </si>
-  <si>
     <t>{typTitle}</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>{urlTitle}</t>
   </si>
   <si>
-    <t>{oeffnungszeitenTitle}</t>
-  </si>
-  <si>
     <t>{babyTitle}</t>
   </si>
   <si>
@@ -175,6 +166,90 @@
   </si>
   <si>
     <t>{gueltigBis}</t>
+  </si>
+  <si>
+    <t>{traegerschaftEmailTitle}</t>
+  </si>
+  <si>
+    <t>{traegerschaftEmail}</t>
+  </si>
+  <si>
+    <t>{familienportalEmailTitle}</t>
+  </si>
+  <si>
+    <t>{familienportalEmail}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBonTitle}</t>
+  </si>
+  <si>
+    <t>{emailBencharichtigungKiBon}</t>
+  </si>
+  <si>
+    <t>{gemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{bfsGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{bfsGemeinde}</t>
+  </si>
+  <si>
+    <t>{oeffnungstageProJahrTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungstageProJahr}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitAbTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitAb}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitBisTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungszeitBis}</t>
+  </si>
+  <si>
+    <t>{ausserordentlicheOeffnungszeitenTitle}</t>
+  </si>
+  <si>
+    <t>{ausserordentlicheOeffnungszeiten}</t>
+  </si>
+  <si>
+    <t>{summePensumWarteliste}</t>
+  </si>
+  <si>
+    <t>{anzahlKinderWartelisteTitle}</t>
+  </si>
+  <si>
+    <t>{anzahlKinderWarteliste}</t>
+  </si>
+  <si>
+    <t>{auslastungTitle}</t>
+  </si>
+  <si>
+    <t>{auslastung}</t>
+  </si>
+  <si>
+    <t>{summePensumWartelisteTitle}</t>
+  </si>
+  <si>
+    <t>{dauerWartelisteTitle}</t>
+  </si>
+  <si>
+    <t>{dauerWarteliste}</t>
+  </si>
+  <si>
+    <t>{grundSchliessungTitle}</t>
+  </si>
+  <si>
+    <t>{grundSchliessung}</t>
   </si>
 </sst>
 </file>
@@ -239,12 +314,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -568,181 +640,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S4" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="13" width="33.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" customWidth="1"/>
-    <col min="17" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="22" width="24.7109375" customWidth="1"/>
-    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="2" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" customWidth="1"/>
+    <col min="11" max="13" width="27.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="20" width="33.5703125" customWidth="1"/>
+    <col min="21" max="22" width="20.140625" customWidth="1"/>
+    <col min="23" max="23" width="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" customWidth="1"/>
+    <col min="26" max="27" width="13.140625" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" customWidth="1"/>
+    <col min="29" max="29" width="15" customWidth="1"/>
+    <col min="30" max="30" width="11" customWidth="1"/>
+    <col min="31" max="31" width="24.7109375" customWidth="1"/>
+    <col min="32" max="32" width="17" customWidth="1"/>
+    <col min="33" max="33" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="K4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="5" t="s">
+      <c r="AB5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="5" t="s">
+      <c r="AC5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="AD5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="AE5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="AF5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>19</v>
+      <c r="AG5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2046: add new fields to institutionen statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67AAF81-4436-45FA-8B08-40A31AFE7406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE270E7-F2F9-4CC1-BE21-0D455B93F3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -183,9 +183,6 @@
     <t>{emailBenachrichtigungKiBonTitle}</t>
   </si>
   <si>
-    <t>{emailBencharichtigungKiBon}</t>
-  </si>
-  <si>
     <t>{gemeindeTitle}</t>
   </si>
   <si>
@@ -250,6 +247,12 @@
   </si>
   <si>
     <t>{grundSchliessung}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBon}</t>
+  </si>
+  <si>
+    <t>{repeatInstitutionenRow}</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -326,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -640,17 +646,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S4" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="6" width="22" customWidth="1"/>
+    <col min="4" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" customWidth="1"/>
@@ -661,25 +668,27 @@
     <col min="21" max="22" width="20.140625" customWidth="1"/>
     <col min="23" max="23" width="38" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="24.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" customWidth="1"/>
-    <col min="26" max="27" width="13.140625" customWidth="1"/>
-    <col min="28" max="28" width="10.42578125" customWidth="1"/>
-    <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="24.7109375" customWidth="1"/>
-    <col min="32" max="32" width="17" customWidth="1"/>
-    <col min="33" max="33" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -714,10 +723,10 @@
         <v>21</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>22</v>
@@ -726,7 +735,7 @@
         <v>23</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>37</v>
@@ -738,16 +747,16 @@
         <v>43</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>40</v>
@@ -777,19 +786,19 @@
         <v>30</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AJ4" s="5" t="s">
-        <v>69</v>
-      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -806,7 +815,7 @@
         <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -824,10 +833,10 @@
         <v>8</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>9</v>
@@ -836,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>38</v>
@@ -848,16 +857,16 @@
         <v>44</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>39</v>
@@ -880,23 +889,26 @@
       <c r="AD5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AE5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="AF5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="AG5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AH5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI5" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2046: add ausserordentliche oeffnungszeiten to institutionen statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE270E7-F2F9-4CC1-BE21-0D455B93F3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943F51DD-F81B-4CB5-B6F9-B8B671A83AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -213,12 +213,6 @@
     <t>{oeffnungszeitBis}</t>
   </si>
   <si>
-    <t>{ausserordentlicheOeffnungszeitenTitle}</t>
-  </si>
-  <si>
-    <t>{ausserordentlicheOeffnungszeiten}</t>
-  </si>
-  <si>
     <t>{summePensumWarteliste}</t>
   </si>
   <si>
@@ -253,6 +247,30 @@
   </si>
   <si>
     <t>{repeatInstitutionenRow}</t>
+  </si>
+  <si>
+    <t>{oeffnungAnWochenenden}</t>
+  </si>
+  <si>
+    <t>{uebernachtungMoeglich}</t>
+  </si>
+  <si>
+    <t>{uebernachtungMoeglichTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungAnWochenendenTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungVorTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungVor}</t>
+  </si>
+  <si>
+    <t>{oeffnungNachTitle}</t>
+  </si>
+  <si>
+    <t>{oeffnungNach}</t>
   </si>
 </sst>
 </file>
@@ -646,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,30 +683,30 @@
     <col min="11" max="13" width="27.85546875" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="20" width="33.5703125" customWidth="1"/>
-    <col min="21" max="22" width="20.140625" customWidth="1"/>
-    <col min="23" max="23" width="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.5703125" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.42578125" customWidth="1"/>
+    <col min="21" max="24" width="20.140625" customWidth="1"/>
+    <col min="25" max="26" width="38" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.5703125" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -747,7 +765,7 @@
         <v>43</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>56</v>
@@ -756,49 +774,58 @@
         <v>58</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="X4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="AB4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="AC4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA4" s="5" t="s">
+      <c r="AD4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AE4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AC4" s="5" t="s">
+      <c r="AF4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AD4" s="5" t="s">
+      <c r="AG4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="5" t="s">
+      <c r="AH4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AI4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AH4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ4" s="5" t="s">
-        <v>68</v>
+      <c r="AM4" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -815,7 +842,7 @@
         <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -857,7 +884,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>57</v>
@@ -866,49 +893,58 @@
         <v>59</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="X5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AH5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AF5" s="6" t="s">
+      <c r="AI5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AG5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH5" s="6" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AK5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AJ5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK5" s="6" t="s">
-        <v>73</v>
+      <c r="AL5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2046: change date formats to decimals where necessary
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943F51DD-F81B-4CB5-B6F9-B8B671A83AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5B3F4-7DF9-4DDE-86B9-311D6538E938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -350,6 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -666,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
   <dimension ref="A1:AN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,16 +932,16 @@
       <c r="AI5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AJ5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AK5" s="6" t="s">
+      <c r="AK5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AL5" s="6" t="s">
+      <c r="AL5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AM5" s="6" t="s">
+      <c r="AM5" s="8" t="s">
         <v>67</v>
       </c>
       <c r="AN5" s="6" t="s">

</xml_diff>

<commit_message>
KIBON-2046: erinnerungmail in statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA5B3F4-7DF9-4DDE-86B9-311D6538E938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A62CBAB-10AB-495B-AA6B-B3B9F0F29CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>{oeffnungNach}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBonMail}</t>
+  </si>
+  <si>
+    <t>{emailBenachrichtigungKiBonMailTitle}</t>
   </si>
 </sst>
 </file>
@@ -308,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -331,11 +337,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -351,6 +379,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -665,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:AN5"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,37 +707,38 @@
     <col min="2" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" customWidth="1"/>
-    <col min="11" max="13" width="27.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="20" width="33.5703125" customWidth="1"/>
-    <col min="21" max="24" width="20.140625" customWidth="1"/>
-    <col min="25" max="26" width="38" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.5703125" customWidth="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="12" max="14" width="27.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="21" width="33.5703125" customWidth="1"/>
+    <col min="22" max="25" width="20.140625" customWidth="1"/>
+    <col min="26" max="27" width="38" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.5703125" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -727,106 +758,109 @@
         <v>49</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="X4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="Y4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Z4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="AA4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AA4" s="5" t="s">
+      <c r="AB4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AC4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AC4" s="5" t="s">
+      <c r="AD4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AD4" s="5" t="s">
+      <c r="AE4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="5" t="s">
+      <c r="AF4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AG4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AH4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AH4" s="5" t="s">
+      <c r="AI4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AI4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AJ4" s="5" t="s">
+      <c r="AK4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AK4" s="5" t="s">
+      <c r="AL4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AL4" s="5" t="s">
+      <c r="AM4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AM4" s="5" t="s">
+      <c r="AN4" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -846,105 +880,108 @@
         <v>70</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AH5" s="7" t="s">
+      <c r="AI5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AK5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AL5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AL5" s="8" t="s">
+      <c r="AM5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AM5" s="8" t="s">
+      <c r="AN5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AN5" s="6" t="s">
+      <c r="AO5" s="10" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2266: Neue Spalte für Standortgemeinde + Gemeindespalte in Trägerschaftgemeinde umbenennt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\kibon-app\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A62CBAB-10AB-495B-AA6B-B3B9F0F29CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB9FCA-05CD-4935-9FF7-F7EA7DB0D959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -183,12 +183,6 @@
     <t>{emailBenachrichtigungKiBonTitle}</t>
   </si>
   <si>
-    <t>{gemeindeTitle}</t>
-  </si>
-  <si>
-    <t>{gemeinde}</t>
-  </si>
-  <si>
     <t>{bfsGemeindeTitle}</t>
   </si>
   <si>
@@ -277,6 +271,15 @@
   </si>
   <si>
     <t>{emailBenachrichtigungKiBonMailTitle}</t>
+  </si>
+  <si>
+    <t>{standortgemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{traegergemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{traegergemeinde}</t>
   </si>
 </sst>
 </file>
@@ -695,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:AO5"/>
+  <dimension ref="A1:AP5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,33 +715,33 @@
     <col min="9" max="9" width="22.85546875" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" customWidth="1"/>
     <col min="11" max="11" width="4.85546875" customWidth="1"/>
-    <col min="12" max="14" width="27.85546875" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="21" width="33.5703125" customWidth="1"/>
-    <col min="22" max="25" width="20.140625" customWidth="1"/>
-    <col min="26" max="27" width="38" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.5703125" customWidth="1"/>
-    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" customWidth="1"/>
+    <col min="12" max="15" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="22" width="33.5703125" customWidth="1"/>
+    <col min="23" max="26" width="20.140625" customWidth="1"/>
+    <col min="27" max="28" width="38" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.5703125" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -758,7 +761,7 @@
         <v>49</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>31</v>
@@ -776,91 +779,94 @@
         <v>21</v>
       </c>
       <c r="M4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="P4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="S4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="W4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="5" t="s">
+      <c r="X4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="X4" s="5" t="s">
+      <c r="Y4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Y4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="AA4" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AB4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AC4" s="5" t="s">
+      <c r="AD4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AD4" s="5" t="s">
+      <c r="AE4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AE4" s="5" t="s">
+      <c r="AF4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AG4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AH4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AH4" s="5" t="s">
+      <c r="AI4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AI4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AJ4" s="5" t="s">
+      <c r="AK4" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="AK4" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="AL4" s="5" t="s">
         <v>61</v>
       </c>
       <c r="AM4" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="AN4" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="AO4" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -877,10 +883,10 @@
         <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>32</v>
@@ -898,79 +904,79 @@
         <v>8</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="P5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="2" t="s">
+      <c r="S5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="W5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="X5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="AA5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AI5" s="7" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AK5" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="AK5" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="AL5" s="8" t="s">
         <v>62</v>
@@ -978,11 +984,14 @@
       <c r="AM5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO5" s="10" t="s">
-        <v>71</v>
+      <c r="AN5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP5" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2266: Standortgemeinde wird nicht mehr von Ort geholt sondern von BFS Gemeinde
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\kibon-app\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FB9FCA-05CD-4935-9FF7-F7EA7DB0D959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59094475-2319-423A-8BDA-DC2EA35C8622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>{traegergemeinde}</t>
+  </si>
+  <si>
+    <t>{standortgemeinde}</t>
   </si>
 </sst>
 </file>
@@ -701,7 +704,7 @@
   <dimension ref="A1:AP5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +907,7 @@
         <v>8</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
KIBON-2432: add status to Institutionen.xlsx statistik, filter anmeldungen-institutionen in statistik view
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\kibon-app\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59094475-2319-423A-8BDA-DC2EA35C8622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6603586F-F206-4315-B461-3073E7438569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>{standortgemeinde}</t>
+  </si>
+  <si>
+    <t>{statusTitle}</t>
+  </si>
+  <si>
+    <t>{status}</t>
   </si>
 </sst>
 </file>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:AP5"/>
+  <dimension ref="A1:AQ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,37 +720,37 @@
     <col min="4" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" customWidth="1"/>
-    <col min="12" max="15" width="27.85546875" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="22" width="33.5703125" customWidth="1"/>
-    <col min="23" max="26" width="20.140625" customWidth="1"/>
-    <col min="27" max="28" width="38" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.5703125" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.42578125" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" customWidth="1"/>
+    <col min="13" max="16" width="27.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="18" max="23" width="33.5703125" customWidth="1"/>
+    <col min="24" max="27" width="20.140625" customWidth="1"/>
+    <col min="28" max="29" width="38" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.5703125" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -770,106 +776,109 @@
         <v>31</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="X4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="Y4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Z4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="AA4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AA4" s="5" t="s">
+      <c r="AB4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AC4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AC4" s="5" t="s">
+      <c r="AD4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AD4" s="5" t="s">
+      <c r="AE4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AE4" s="5" t="s">
+      <c r="AF4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AG4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AH4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AH4" s="5" t="s">
+      <c r="AI4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AI4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AJ4" s="5" t="s">
+      <c r="AK4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AK4" s="5" t="s">
+      <c r="AL4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AL4" s="5" t="s">
+      <c r="AM4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AM4" s="5" t="s">
+      <c r="AN4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AN4" s="5" t="s">
+      <c r="AO4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AO4" s="5" t="s">
+      <c r="AP4" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -895,105 +904,108 @@
         <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="V5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AD5" s="3" t="s">
+      <c r="AE5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AJ5" s="7" t="s">
+      <c r="AK5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AK5" s="6" t="s">
+      <c r="AL5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AL5" s="8" t="s">
+      <c r="AM5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AM5" s="8" t="s">
+      <c r="AN5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN5" s="8" t="s">
+      <c r="AO5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AO5" s="9" t="s">
+      <c r="AP5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="AP5" s="10" t="s">
+      <c r="AQ5" s="10" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2480: Add BFS Nr. Standortgemeinde to Institutionen Statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Institutionen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6603586F-F206-4315-B461-3073E7438569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3165087C-D53F-444A-B151-C7BEB18539C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{617232BA-F9C5-4529-BA67-503720E5A6AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>{emailTitle}</t>
   </si>
@@ -183,12 +183,6 @@
     <t>{emailBenachrichtigungKiBonTitle}</t>
   </si>
   <si>
-    <t>{bfsGemeindeTitle}</t>
-  </si>
-  <si>
-    <t>{bfsGemeinde}</t>
-  </si>
-  <si>
     <t>{oeffnungstageProJahrTitle}</t>
   </si>
   <si>
@@ -289,6 +283,18 @@
   </si>
   <si>
     <t>{status}</t>
+  </si>
+  <si>
+    <t>{bfsStandortgemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{bfsTraegergemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{bfsTraegergemeinde}</t>
+  </si>
+  <si>
+    <t>{bfsStandortgemeinde}</t>
   </si>
 </sst>
 </file>
@@ -707,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B88504-77C9-47C6-9364-CB212A99C694}">
-  <dimension ref="A1:AQ5"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,33 +730,33 @@
     <col min="10" max="10" width="22.85546875" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" customWidth="1"/>
     <col min="12" max="12" width="4.85546875" customWidth="1"/>
-    <col min="13" max="16" width="27.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="18" max="23" width="33.5703125" customWidth="1"/>
-    <col min="24" max="27" width="20.140625" customWidth="1"/>
-    <col min="28" max="29" width="38" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.5703125" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.42578125" customWidth="1"/>
+    <col min="13" max="17" width="27.85546875" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="19" max="24" width="33.5703125" customWidth="1"/>
+    <col min="25" max="28" width="20.140625" customWidth="1"/>
+    <col min="29" max="30" width="38" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.5703125" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -770,13 +776,13 @@
         <v>49</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>33</v>
@@ -791,94 +797,97 @@
         <v>21</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="5" t="s">
+      <c r="U4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4" s="5" t="s">
+      <c r="Z4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Y4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4" s="5" t="s">
+      <c r="AA4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AA4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB4" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="AC4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AE4" s="5" t="s">
+      <c r="AF4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AG4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AG4" s="5" t="s">
+      <c r="AH4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AH4" s="5" t="s">
+      <c r="AI4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AI4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AJ4" s="5" t="s">
+      <c r="AK4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AK4" s="5" t="s">
+      <c r="AL4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AL4" s="5" t="s">
+      <c r="AM4" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="AM4" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="AN4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="AO4" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AP4" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="AQ4" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -895,16 +904,16 @@
         <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>34</v>
@@ -919,82 +928,82 @@
         <v>8</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="P5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="2" t="s">
+      <c r="U5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="T5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="X5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Y5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AA5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AC5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AD5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AK5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AK5" s="7" t="s">
+      <c r="AL5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AL5" s="6" t="s">
+      <c r="AM5" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="AM5" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="AN5" s="8" t="s">
         <v>60</v>
@@ -1002,11 +1011,14 @@
       <c r="AO5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AP5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ5" s="10" t="s">
-        <v>69</v>
+      <c r="AP5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR5" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>